<commit_message>
Fixed file opening issues
</commit_message>
<xml_diff>
--- a/PackagingPlusInvoices.xlsx
+++ b/PackagingPlusInvoices.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet sheetId="1" name="453543" state="visible" r:id="rId4"/>
     <sheet sheetId="2" name="Jul2020" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Aug2020" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -854,6 +855,96 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <f>SUM(B2:B2)</f>
+      </c>
+      <c r="C3">
+        <f>SUM(C2:C2)</f>
+      </c>
+      <c r="D3">
+        <f>SUM(D2:D2)</f>
+      </c>
+      <c r="E3">
+        <f>SUM(E2:E2)</f>
+      </c>
+      <c r="F3">
+        <f>SUM(F2:F2)</f>
+      </c>
+      <c r="G3">
+        <f>SUM(G2:G2)</f>
+      </c>
+      <c r="H3">
+        <f>SUM(H2:H2)</f>
+      </c>
+      <c r="I3">
+        <f>SUM(I2:I2)</f>
+      </c>
+      <c r="J3">
+        <f>SUM(J2:J2)</f>
+      </c>
+      <c r="K3">
+        <f>SUM(K2:K2)</f>
+      </c>
+      <c r="L3">
+        <f>SUM(L2:L2)</f>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>